<commit_message>
[Silverfox] 앱노말 FX 색상 기조
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/Abnormal_Type.xlsx
+++ b/DesignDocs/Design/Abnormal_Type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FC9C1D-000D-43FB-B3E3-30BA89529537}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7479D5FC-CB06-4E99-BF34-EB8DE91E6289}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -366,6 +366,38 @@
   </si>
   <si>
     <t>{(poison, 15, 5, 5, all)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대표 색상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>녹색 계열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보라색 계열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검은색 계열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연두색 계열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분홍색 계열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노란색 계열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주황색 계열</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -769,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L19"/>
+  <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -786,10 +818,11 @@
     <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="43.5" customWidth="1"/>
     <col min="12" max="12" width="51.75" customWidth="1"/>
+    <col min="13" max="13" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
@@ -823,8 +856,11 @@
       <c r="L2" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="M2" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>60</v>
       </c>
@@ -852,8 +888,11 @@
       <c r="L3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>61</v>
       </c>
@@ -875,8 +914,9 @@
       <c r="L4" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>62</v>
       </c>
@@ -900,8 +940,11 @@
       <c r="L5" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>63</v>
       </c>
@@ -923,8 +966,9 @@
       <c r="L6" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>64</v>
       </c>
@@ -946,8 +990,9 @@
       <c r="L7" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>65</v>
       </c>
@@ -969,8 +1014,9 @@
       <c r="L8" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>66</v>
       </c>
@@ -992,8 +1038,11 @@
       <c r="L9" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>67</v>
       </c>
@@ -1015,8 +1064,9 @@
       <c r="L10" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>68</v>
       </c>
@@ -1042,8 +1092,11 @@
       <c r="L11" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>69</v>
       </c>
@@ -1071,8 +1124,11 @@
       <c r="L12" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>70</v>
       </c>
@@ -1102,8 +1158,11 @@
       <c r="L13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>71</v>
       </c>
@@ -1131,8 +1190,9 @@
       <c r="L14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>72</v>
       </c>
@@ -1160,8 +1220,9 @@
       <c r="L15" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>73</v>
       </c>
@@ -1189,8 +1250,9 @@
       <c r="L16" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>74</v>
       </c>
@@ -1218,8 +1280,9 @@
       <c r="L17" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>75</v>
       </c>
@@ -1247,8 +1310,11 @@
       <c r="L18" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="M18" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="33" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>76</v>
       </c>
@@ -1276,6 +1342,7 @@
       <c r="L19" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="M19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>